<commit_message>
added com1 and com2 pins
</commit_message>
<xml_diff>
--- a/board/crossBar.xlsx
+++ b/board/crossBar.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1841" uniqueCount="285">
   <si>
     <t>AF0</t>
   </si>
@@ -66,9 +66,6 @@
     <t>TIM5_CH4</t>
   </si>
   <si>
-    <t>USART4_CTS</t>
-  </si>
-  <si>
     <t>EVENT OUT</t>
   </si>
   <si>
@@ -862,6 +859,18 @@
   </si>
   <si>
     <t>IMEAS_RELAY_3</t>
+  </si>
+  <si>
+    <t>COM1_TX</t>
+  </si>
+  <si>
+    <t>COM1_RX</t>
+  </si>
+  <si>
+    <t>COM2_TX</t>
+  </si>
+  <si>
+    <t>COM2_RX</t>
   </si>
 </sst>
 </file>
@@ -1212,12 +1221,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C78" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C81" activePane="bottomRight" state="frozen"/>
       <selection activeCell="G2" sqref="G2"/>
       <selection pane="topRight" activeCell="G2" sqref="G2"/>
       <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
-      <selection pane="bottomRight" activeCell="F85" sqref="F85"/>
+      <selection pane="bottomRight" activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,7 +1257,7 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -1275,75 +1284,75 @@
         <v>8</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>10</v>
@@ -1360,11 +1369,11 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" t="s">
         <v>76</v>
       </c>
-      <c r="E3" t="s">
-        <v>77</v>
-      </c>
       <c r="F3" t="s">
         <v>10</v>
       </c>
@@ -1378,7 +1387,7 @@
         <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K3" t="s">
         <v>10</v>
@@ -1408,7 +1417,7 @@
         <v>10</v>
       </c>
       <c r="T3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -1416,11 +1425,11 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" t="s">
         <v>78</v>
       </c>
-      <c r="E4" t="s">
-        <v>79</v>
-      </c>
       <c r="F4" t="s">
         <v>10</v>
       </c>
@@ -1464,7 +1473,7 @@
         <v>10</v>
       </c>
       <c r="T4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -1472,10 +1481,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
@@ -1490,7 +1499,7 @@
         <v>10</v>
       </c>
       <c r="J5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K5" t="s">
         <v>10</v>
@@ -1520,7 +1529,7 @@
         <v>10</v>
       </c>
       <c r="T5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -1528,16 +1537,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
@@ -1546,13 +1555,13 @@
         <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I6" t="s">
         <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K6" t="s">
         <v>10</v>
@@ -1582,7 +1591,7 @@
         <v>10</v>
       </c>
       <c r="T6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -1590,25 +1599,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" t="s">
         <v>81</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
         <v>82</v>
       </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" t="s">
-        <v>83</v>
-      </c>
       <c r="I7" t="s">
         <v>10</v>
       </c>
       <c r="J7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K7" t="s">
         <v>10</v>
@@ -1638,7 +1647,7 @@
         <v>10</v>
       </c>
       <c r="T7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -1646,10 +1655,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" t="s">
         <v>92</v>
-      </c>
-      <c r="C8" t="s">
-        <v>93</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -1705,7 +1714,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -1753,7 +1762,7 @@
         <v>10</v>
       </c>
       <c r="T9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -1761,7 +1770,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -1809,7 +1818,7 @@
         <v>10</v>
       </c>
       <c r="T10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -1817,7 +1826,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1865,7 +1874,7 @@
         <v>10</v>
       </c>
       <c r="T11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1873,10 +1882,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>10</v>
@@ -1932,10 +1941,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>10</v>
@@ -2168,7 +2177,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>10</v>
@@ -2216,7 +2225,7 @@
         <v>10</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2224,7 +2233,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>10</v>
@@ -2272,7 +2281,7 @@
         <v>10</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2280,7 +2289,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>10</v>
@@ -2298,10 +2307,10 @@
         <v>10</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>10</v>
@@ -2336,7 +2345,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>10</v>
@@ -2354,7 +2363,7 @@
         <v>10</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>10</v>
@@ -2392,10 +2401,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>10</v>
@@ -2451,10 +2460,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>10</v>
@@ -2510,10 +2519,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -2569,10 +2578,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -2634,10 +2643,10 @@
         <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H25" t="s">
         <v>10</v>
@@ -2652,7 +2661,7 @@
         <v>10</v>
       </c>
       <c r="L25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M25" t="s">
         <v>10</v>
@@ -2676,7 +2685,7 @@
         <v>10</v>
       </c>
       <c r="T25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
@@ -2684,16 +2693,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
       </c>
       <c r="F26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H26" t="s">
         <v>10</v>
@@ -2708,7 +2717,7 @@
         <v>10</v>
       </c>
       <c r="L26" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M26" t="s">
         <v>10</v>
@@ -2732,7 +2741,7 @@
         <v>10</v>
       </c>
       <c r="T26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
@@ -2740,19 +2749,25 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>99</v>
+        <v>98</v>
+      </c>
+      <c r="C27" t="s">
+        <v>283</v>
+      </c>
+      <c r="D27" t="s">
+        <v>177</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
       </c>
       <c r="F27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I27" t="s">
         <v>10</v>
@@ -2764,7 +2779,7 @@
         <v>10</v>
       </c>
       <c r="L27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M27" t="s">
         <v>10</v>
@@ -2788,7 +2803,7 @@
         <v>10</v>
       </c>
       <c r="T27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
@@ -2796,25 +2811,25 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C28" t="s">
-        <v>267</v>
+        <v>284</v>
       </c>
       <c r="D28" t="s">
-        <v>226</v>
+        <v>176</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
       </c>
       <c r="F28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G28" t="s">
         <v>15</v>
       </c>
       <c r="H28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I28" t="s">
         <v>10</v>
@@ -2826,7 +2841,7 @@
         <v>10</v>
       </c>
       <c r="L28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M28" t="s">
         <v>10</v>
@@ -2850,7 +2865,7 @@
         <v>10</v>
       </c>
       <c r="T28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
@@ -2858,10 +2873,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -2917,10 +2932,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -2976,9 +2991,14 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>266</v>
+      </c>
+      <c r="D31" t="s">
+        <v>225</v>
+      </c>
       <c r="E31" t="s">
         <v>10</v>
       </c>
@@ -2995,13 +3015,13 @@
         <v>10</v>
       </c>
       <c r="J31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K31" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M31" t="s">
         <v>10</v>
@@ -3025,7 +3045,7 @@
         <v>10</v>
       </c>
       <c r="T31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
@@ -3033,19 +3053,19 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32" t="s">
+        <v>267</v>
+      </c>
+      <c r="D32" t="s">
         <v>268</v>
       </c>
-      <c r="D32" t="s">
-        <v>269</v>
-      </c>
       <c r="E32" t="s">
         <v>10</v>
       </c>
       <c r="F32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G32" t="s">
         <v>10</v>
@@ -3057,7 +3077,7 @@
         <v>10</v>
       </c>
       <c r="J32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K32" t="s">
         <v>10</v>
@@ -3087,7 +3107,7 @@
         <v>10</v>
       </c>
       <c r="T32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
@@ -3095,19 +3115,19 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E33" t="s">
         <v>10</v>
       </c>
       <c r="F33" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G33" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H33" t="s">
         <v>10</v>
@@ -3116,7 +3136,7 @@
         <v>10</v>
       </c>
       <c r="J33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K33" t="s">
         <v>10</v>
@@ -3146,7 +3166,7 @@
         <v>10</v>
       </c>
       <c r="T33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
@@ -3154,22 +3174,22 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E34" t="s">
         <v>10</v>
       </c>
       <c r="F34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G34" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H34" t="s">
         <v>10</v>
@@ -3178,7 +3198,7 @@
         <v>10</v>
       </c>
       <c r="J34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K34" t="s">
         <v>10</v>
@@ -3208,7 +3228,7 @@
         <v>10</v>
       </c>
       <c r="T34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
@@ -3216,13 +3236,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C35" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D35" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
@@ -3270,7 +3290,7 @@
         <v>10</v>
       </c>
       <c r="T35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
@@ -3278,13 +3298,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C36" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D36" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
@@ -3332,7 +3352,7 @@
         <v>10</v>
       </c>
       <c r="T36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
@@ -3340,22 +3360,22 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D37" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E37" t="s">
         <v>10</v>
       </c>
       <c r="F37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G37" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H37" t="s">
         <v>10</v>
@@ -3394,7 +3414,7 @@
         <v>10</v>
       </c>
       <c r="T37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
@@ -3402,16 +3422,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E38" t="s">
         <v>10</v>
       </c>
       <c r="F38" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G38" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H38" t="s">
         <v>10</v>
@@ -3450,7 +3470,7 @@
         <v>10</v>
       </c>
       <c r="T38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
@@ -3458,10 +3478,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C39" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E39" t="s">
         <v>10</v>
@@ -3479,7 +3499,7 @@
         <v>10</v>
       </c>
       <c r="J39" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K39" t="s">
         <v>10</v>
@@ -3509,7 +3529,7 @@
         <v>10</v>
       </c>
       <c r="T39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
@@ -3517,13 +3537,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E40" t="s">
         <v>10</v>
       </c>
       <c r="F40" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G40" t="s">
         <v>10</v>
@@ -3565,7 +3585,7 @@
         <v>10</v>
       </c>
       <c r="T40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
@@ -3573,13 +3593,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E41" t="s">
         <v>10</v>
       </c>
       <c r="F41" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G41" t="s">
         <v>10</v>
@@ -3621,7 +3641,7 @@
         <v>10</v>
       </c>
       <c r="T41" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
@@ -3629,13 +3649,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E42" t="s">
         <v>10</v>
       </c>
       <c r="F42" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G42" t="s">
         <v>10</v>
@@ -3677,7 +3697,7 @@
         <v>10</v>
       </c>
       <c r="T42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
@@ -3685,13 +3705,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E43" t="s">
         <v>10</v>
       </c>
       <c r="F43" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G43" t="s">
         <v>10</v>
@@ -3733,7 +3753,7 @@
         <v>10</v>
       </c>
       <c r="T43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
@@ -3741,13 +3761,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E44" t="s">
         <v>10</v>
       </c>
       <c r="F44" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G44" t="s">
         <v>10</v>
@@ -3759,7 +3779,7 @@
         <v>10</v>
       </c>
       <c r="J44" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K44" t="s">
         <v>10</v>
@@ -3789,7 +3809,7 @@
         <v>10</v>
       </c>
       <c r="T44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
@@ -3797,13 +3817,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E45" t="s">
         <v>10</v>
       </c>
       <c r="F45" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G45" t="s">
         <v>10</v>
@@ -3815,7 +3835,7 @@
         <v>10</v>
       </c>
       <c r="J45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K45" t="s">
         <v>10</v>
@@ -3845,7 +3865,7 @@
         <v>10</v>
       </c>
       <c r="T45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
@@ -3853,13 +3873,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E46" t="s">
         <v>10</v>
       </c>
       <c r="F46" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G46" t="s">
         <v>10</v>
@@ -3871,7 +3891,7 @@
         <v>10</v>
       </c>
       <c r="J46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K46" t="s">
         <v>10</v>
@@ -3901,7 +3921,7 @@
         <v>10</v>
       </c>
       <c r="T46" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
@@ -3909,13 +3929,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E47" t="s">
         <v>10</v>
       </c>
       <c r="F47" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G47" t="s">
         <v>10</v>
@@ -3927,7 +3947,7 @@
         <v>10</v>
       </c>
       <c r="J47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K47" t="s">
         <v>10</v>
@@ -3957,7 +3977,7 @@
         <v>10</v>
       </c>
       <c r="T47" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
@@ -3965,13 +3985,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E48" t="s">
         <v>10</v>
       </c>
       <c r="F48" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G48" t="s">
         <v>10</v>
@@ -4013,7 +4033,7 @@
         <v>10</v>
       </c>
       <c r="T48" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
@@ -4021,19 +4041,19 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C49" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D49" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E49" t="s">
         <v>10</v>
       </c>
       <c r="F49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G49" t="s">
         <v>10</v>
@@ -4042,10 +4062,10 @@
         <v>10</v>
       </c>
       <c r="I49" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J49" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K49" t="s">
         <v>10</v>
@@ -4075,7 +4095,7 @@
         <v>10</v>
       </c>
       <c r="T49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
@@ -4083,10 +4103,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C50" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E50" t="s">
         <v>10</v>
@@ -4142,10 +4162,10 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C51" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E51" t="s">
         <v>10</v>
@@ -4201,10 +4221,10 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E52" t="s">
         <v>10</v>
@@ -4260,19 +4280,19 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C53" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D53" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E53" t="s">
         <v>10</v>
       </c>
       <c r="F53" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G53" t="s">
         <v>10</v>
@@ -4281,10 +4301,10 @@
         <v>10</v>
       </c>
       <c r="I53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J53" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K53" t="s">
         <v>10</v>
@@ -4314,7 +4334,7 @@
         <v>10</v>
       </c>
       <c r="T53" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
@@ -4322,13 +4342,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E54" t="s">
         <v>10</v>
       </c>
       <c r="F54" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G54" t="s">
         <v>10</v>
@@ -4340,7 +4360,7 @@
         <v>10</v>
       </c>
       <c r="J54" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K54" t="s">
         <v>10</v>
@@ -4370,7 +4390,7 @@
         <v>10</v>
       </c>
       <c r="T54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
@@ -4378,13 +4398,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E55" t="s">
         <v>10</v>
       </c>
       <c r="F55" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G55" t="s">
         <v>10</v>
@@ -4396,10 +4416,10 @@
         <v>10</v>
       </c>
       <c r="J55" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K55" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L55" t="s">
         <v>10</v>
@@ -4426,7 +4446,7 @@
         <v>10</v>
       </c>
       <c r="T55" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
@@ -4434,19 +4454,19 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C56" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D56" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E56" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F56" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G56" t="s">
         <v>10</v>
@@ -4458,7 +4478,7 @@
         <v>10</v>
       </c>
       <c r="J56" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K56" t="s">
         <v>10</v>
@@ -4488,7 +4508,7 @@
         <v>10</v>
       </c>
       <c r="T56" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
@@ -4496,7 +4516,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E57" t="s">
         <v>10</v>
@@ -4544,7 +4564,7 @@
         <v>10</v>
       </c>
       <c r="T57" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
@@ -4552,7 +4572,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E58" t="s">
         <v>10</v>
@@ -4600,7 +4620,7 @@
         <v>10</v>
       </c>
       <c r="T58" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
@@ -4608,7 +4628,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E59" t="s">
         <v>10</v>
@@ -4653,7 +4673,7 @@
         <v>10</v>
       </c>
       <c r="T59" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
@@ -4661,7 +4681,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E60" t="s">
         <v>10</v>
@@ -4709,7 +4729,7 @@
         <v>10</v>
       </c>
       <c r="T60" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
@@ -4717,7 +4737,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E61" t="s">
         <v>10</v>
@@ -4726,7 +4746,7 @@
         <v>10</v>
       </c>
       <c r="G61" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H61" t="s">
         <v>10</v>
@@ -4765,7 +4785,7 @@
         <v>10</v>
       </c>
       <c r="T61" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
@@ -4773,7 +4793,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E62" t="s">
         <v>10</v>
@@ -4782,7 +4802,7 @@
         <v>10</v>
       </c>
       <c r="G62" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H62" t="s">
         <v>10</v>
@@ -4821,7 +4841,7 @@
         <v>10</v>
       </c>
       <c r="T62" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
@@ -4829,7 +4849,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E63" t="s">
         <v>10</v>
@@ -4838,7 +4858,7 @@
         <v>10</v>
       </c>
       <c r="G63" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H63" t="s">
         <v>10</v>
@@ -4877,7 +4897,7 @@
         <v>10</v>
       </c>
       <c r="T63" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
@@ -4885,7 +4905,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E64" t="s">
         <v>10</v>
@@ -4894,7 +4914,7 @@
         <v>10</v>
       </c>
       <c r="G64" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H64" t="s">
         <v>10</v>
@@ -4933,7 +4953,7 @@
         <v>10</v>
       </c>
       <c r="T64" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
@@ -4941,47 +4961,47 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
+        <v>56</v>
+      </c>
+      <c r="E65" t="s">
+        <v>10</v>
+      </c>
+      <c r="F65" t="s">
+        <v>10</v>
+      </c>
+      <c r="G65" t="s">
+        <v>197</v>
+      </c>
+      <c r="H65" t="s">
+        <v>10</v>
+      </c>
+      <c r="I65" t="s">
+        <v>10</v>
+      </c>
+      <c r="J65" t="s">
+        <v>190</v>
+      </c>
+      <c r="K65" t="s">
+        <v>10</v>
+      </c>
+      <c r="L65" t="s">
+        <v>10</v>
+      </c>
+      <c r="M65" t="s">
+        <v>20</v>
+      </c>
+      <c r="N65" t="s">
+        <v>10</v>
+      </c>
+      <c r="O65" t="s">
+        <v>10</v>
+      </c>
+      <c r="P65" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q65" t="s">
         <v>57</v>
       </c>
-      <c r="E65" t="s">
-        <v>10</v>
-      </c>
-      <c r="F65" t="s">
-        <v>10</v>
-      </c>
-      <c r="G65" t="s">
-        <v>198</v>
-      </c>
-      <c r="H65" t="s">
-        <v>10</v>
-      </c>
-      <c r="I65" t="s">
-        <v>10</v>
-      </c>
-      <c r="J65" t="s">
-        <v>191</v>
-      </c>
-      <c r="K65" t="s">
-        <v>10</v>
-      </c>
-      <c r="L65" t="s">
-        <v>10</v>
-      </c>
-      <c r="M65" t="s">
-        <v>21</v>
-      </c>
-      <c r="N65" t="s">
-        <v>10</v>
-      </c>
-      <c r="O65" t="s">
-        <v>10</v>
-      </c>
-      <c r="P65" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q65" t="s">
-        <v>58</v>
-      </c>
       <c r="R65" t="s">
         <v>10</v>
       </c>
@@ -4989,7 +5009,7 @@
         <v>10</v>
       </c>
       <c r="T65" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
@@ -4997,47 +5017,47 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
+        <v>58</v>
+      </c>
+      <c r="E66" t="s">
+        <v>10</v>
+      </c>
+      <c r="F66" t="s">
+        <v>10</v>
+      </c>
+      <c r="G66" t="s">
+        <v>198</v>
+      </c>
+      <c r="H66" t="s">
+        <v>10</v>
+      </c>
+      <c r="I66" t="s">
+        <v>10</v>
+      </c>
+      <c r="J66" t="s">
+        <v>10</v>
+      </c>
+      <c r="K66" t="s">
+        <v>213</v>
+      </c>
+      <c r="L66" t="s">
+        <v>10</v>
+      </c>
+      <c r="M66" t="s">
+        <v>23</v>
+      </c>
+      <c r="N66" t="s">
+        <v>10</v>
+      </c>
+      <c r="O66" t="s">
+        <v>10</v>
+      </c>
+      <c r="P66" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q66" t="s">
         <v>59</v>
       </c>
-      <c r="E66" t="s">
-        <v>10</v>
-      </c>
-      <c r="F66" t="s">
-        <v>10</v>
-      </c>
-      <c r="G66" t="s">
-        <v>199</v>
-      </c>
-      <c r="H66" t="s">
-        <v>10</v>
-      </c>
-      <c r="I66" t="s">
-        <v>10</v>
-      </c>
-      <c r="J66" t="s">
-        <v>10</v>
-      </c>
-      <c r="K66" t="s">
-        <v>214</v>
-      </c>
-      <c r="L66" t="s">
-        <v>10</v>
-      </c>
-      <c r="M66" t="s">
-        <v>24</v>
-      </c>
-      <c r="N66" t="s">
-        <v>10</v>
-      </c>
-      <c r="O66" t="s">
-        <v>10</v>
-      </c>
-      <c r="P66" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q66" t="s">
-        <v>60</v>
-      </c>
       <c r="R66" t="s">
         <v>10</v>
       </c>
@@ -5045,7 +5065,7 @@
         <v>10</v>
       </c>
       <c r="T66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
@@ -5053,47 +5073,47 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
+        <v>60</v>
+      </c>
+      <c r="E67" t="s">
+        <v>10</v>
+      </c>
+      <c r="F67" t="s">
+        <v>10</v>
+      </c>
+      <c r="G67" t="s">
+        <v>202</v>
+      </c>
+      <c r="H67" t="s">
+        <v>10</v>
+      </c>
+      <c r="I67" t="s">
+        <v>10</v>
+      </c>
+      <c r="J67" t="s">
+        <v>10</v>
+      </c>
+      <c r="K67" t="s">
+        <v>10</v>
+      </c>
+      <c r="L67" t="s">
+        <v>10</v>
+      </c>
+      <c r="M67" t="s">
         <v>61</v>
       </c>
-      <c r="E67" t="s">
-        <v>10</v>
-      </c>
-      <c r="F67" t="s">
-        <v>10</v>
-      </c>
-      <c r="G67" t="s">
-        <v>203</v>
-      </c>
-      <c r="H67" t="s">
-        <v>10</v>
-      </c>
-      <c r="I67" t="s">
-        <v>10</v>
-      </c>
-      <c r="J67" t="s">
-        <v>10</v>
-      </c>
-      <c r="K67" t="s">
-        <v>10</v>
-      </c>
-      <c r="L67" t="s">
-        <v>10</v>
-      </c>
-      <c r="M67" t="s">
+      <c r="N67" t="s">
+        <v>10</v>
+      </c>
+      <c r="O67" t="s">
+        <v>10</v>
+      </c>
+      <c r="P67" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q67" t="s">
         <v>62</v>
       </c>
-      <c r="N67" t="s">
-        <v>10</v>
-      </c>
-      <c r="O67" t="s">
-        <v>10</v>
-      </c>
-      <c r="P67" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q67" t="s">
-        <v>63</v>
-      </c>
       <c r="R67" t="s">
         <v>10</v>
       </c>
@@ -5101,7 +5121,7 @@
         <v>10</v>
       </c>
       <c r="T67" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
@@ -5109,22 +5129,22 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E68" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F68" t="s">
         <v>10</v>
       </c>
       <c r="G68" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I68" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J68" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K68" t="s">
         <v>10</v>
@@ -5145,7 +5165,7 @@
         <v>10</v>
       </c>
       <c r="Q68" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R68" t="s">
         <v>10</v>
@@ -5154,7 +5174,7 @@
         <v>10</v>
       </c>
       <c r="T68" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
@@ -5162,47 +5182,47 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
+        <v>35</v>
+      </c>
+      <c r="C69" t="s">
+        <v>269</v>
+      </c>
+      <c r="D69" t="s">
+        <v>156</v>
+      </c>
+      <c r="E69" t="s">
+        <v>144</v>
+      </c>
+      <c r="F69" t="s">
+        <v>156</v>
+      </c>
+      <c r="G69" t="s">
+        <v>10</v>
+      </c>
+      <c r="H69" t="s">
+        <v>10</v>
+      </c>
+      <c r="I69" t="s">
+        <v>200</v>
+      </c>
+      <c r="J69" t="s">
+        <v>10</v>
+      </c>
+      <c r="K69" t="s">
+        <v>10</v>
+      </c>
+      <c r="L69" t="s">
+        <v>161</v>
+      </c>
+      <c r="M69" t="s">
+        <v>10</v>
+      </c>
+      <c r="N69" t="s">
+        <v>10</v>
+      </c>
+      <c r="O69" t="s">
         <v>36</v>
       </c>
-      <c r="C69" t="s">
-        <v>270</v>
-      </c>
-      <c r="D69" t="s">
-        <v>157</v>
-      </c>
-      <c r="E69" t="s">
-        <v>145</v>
-      </c>
-      <c r="F69" t="s">
-        <v>157</v>
-      </c>
-      <c r="G69" t="s">
-        <v>10</v>
-      </c>
-      <c r="H69" t="s">
-        <v>10</v>
-      </c>
-      <c r="I69" t="s">
-        <v>201</v>
-      </c>
-      <c r="J69" t="s">
-        <v>10</v>
-      </c>
-      <c r="K69" t="s">
-        <v>10</v>
-      </c>
-      <c r="L69" t="s">
-        <v>162</v>
-      </c>
-      <c r="M69" t="s">
-        <v>10</v>
-      </c>
-      <c r="N69" t="s">
-        <v>10</v>
-      </c>
-      <c r="O69" t="s">
-        <v>37</v>
-      </c>
       <c r="P69" t="s">
         <v>10</v>
       </c>
@@ -5216,7 +5236,7 @@
         <v>10</v>
       </c>
       <c r="T69" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
@@ -5224,47 +5244,47 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
+        <v>37</v>
+      </c>
+      <c r="C70" t="s">
+        <v>232</v>
+      </c>
+      <c r="D70" t="s">
+        <v>160</v>
+      </c>
+      <c r="E70" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" t="s">
+        <v>167</v>
+      </c>
+      <c r="G70" t="s">
+        <v>10</v>
+      </c>
+      <c r="H70" t="s">
+        <v>10</v>
+      </c>
+      <c r="I70" t="s">
+        <v>199</v>
+      </c>
+      <c r="J70" t="s">
+        <v>10</v>
+      </c>
+      <c r="K70" t="s">
+        <v>10</v>
+      </c>
+      <c r="L70" t="s">
+        <v>160</v>
+      </c>
+      <c r="M70" t="s">
+        <v>10</v>
+      </c>
+      <c r="N70" t="s">
+        <v>10</v>
+      </c>
+      <c r="O70" t="s">
         <v>38</v>
       </c>
-      <c r="C70" t="s">
-        <v>233</v>
-      </c>
-      <c r="D70" t="s">
-        <v>161</v>
-      </c>
-      <c r="E70" t="s">
-        <v>10</v>
-      </c>
-      <c r="F70" t="s">
-        <v>168</v>
-      </c>
-      <c r="G70" t="s">
-        <v>10</v>
-      </c>
-      <c r="H70" t="s">
-        <v>10</v>
-      </c>
-      <c r="I70" t="s">
-        <v>200</v>
-      </c>
-      <c r="J70" t="s">
-        <v>10</v>
-      </c>
-      <c r="K70" t="s">
-        <v>10</v>
-      </c>
-      <c r="L70" t="s">
-        <v>161</v>
-      </c>
-      <c r="M70" t="s">
-        <v>10</v>
-      </c>
-      <c r="N70" t="s">
-        <v>10</v>
-      </c>
-      <c r="O70" t="s">
-        <v>39</v>
-      </c>
       <c r="P70" t="s">
         <v>10</v>
       </c>
@@ -5278,7 +5298,7 @@
         <v>10</v>
       </c>
       <c r="T70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
@@ -5286,38 +5306,38 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C71" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D71" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E71" t="s">
         <v>10</v>
       </c>
       <c r="F71" t="s">
+        <v>154</v>
+      </c>
+      <c r="G71" t="s">
+        <v>10</v>
+      </c>
+      <c r="H71" t="s">
+        <v>10</v>
+      </c>
+      <c r="I71" t="s">
+        <v>10</v>
+      </c>
+      <c r="J71" t="s">
+        <v>10</v>
+      </c>
+      <c r="K71" t="s">
+        <v>10</v>
+      </c>
+      <c r="L71" t="s">
         <v>155</v>
       </c>
-      <c r="G71" t="s">
-        <v>10</v>
-      </c>
-      <c r="H71" t="s">
-        <v>10</v>
-      </c>
-      <c r="I71" t="s">
-        <v>10</v>
-      </c>
-      <c r="J71" t="s">
-        <v>10</v>
-      </c>
-      <c r="K71" t="s">
-        <v>10</v>
-      </c>
-      <c r="L71" t="s">
-        <v>156</v>
-      </c>
       <c r="M71" t="s">
         <v>10</v>
       </c>
@@ -5325,7 +5345,7 @@
         <v>10</v>
       </c>
       <c r="O71" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P71" t="s">
         <v>10</v>
@@ -5340,7 +5360,7 @@
         <v>10</v>
       </c>
       <c r="T71" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
@@ -5348,13 +5368,13 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E72" t="s">
         <v>10</v>
       </c>
       <c r="F72" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G72" t="s">
         <v>10</v>
@@ -5372,17 +5392,17 @@
         <v>10</v>
       </c>
       <c r="L72" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M72" t="s">
+        <v>20</v>
+      </c>
+      <c r="N72" t="s">
+        <v>10</v>
+      </c>
+      <c r="O72" t="s">
         <v>21</v>
       </c>
-      <c r="N72" t="s">
-        <v>10</v>
-      </c>
-      <c r="O72" t="s">
-        <v>22</v>
-      </c>
       <c r="P72" t="s">
         <v>10</v>
       </c>
@@ -5396,7 +5416,7 @@
         <v>10</v>
       </c>
       <c r="T72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
@@ -5404,13 +5424,13 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E73" t="s">
         <v>10</v>
       </c>
       <c r="F73" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G73" t="s">
         <v>10</v>
@@ -5428,17 +5448,17 @@
         <v>10</v>
       </c>
       <c r="L73" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M73" t="s">
+        <v>23</v>
+      </c>
+      <c r="N73" t="s">
+        <v>10</v>
+      </c>
+      <c r="O73" t="s">
         <v>24</v>
       </c>
-      <c r="N73" t="s">
-        <v>10</v>
-      </c>
-      <c r="O73" t="s">
-        <v>25</v>
-      </c>
       <c r="P73" t="s">
         <v>10</v>
       </c>
@@ -5452,7 +5472,7 @@
         <v>10</v>
       </c>
       <c r="T73" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
@@ -5460,13 +5480,13 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C74" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E74" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F74" t="s">
         <v>10</v>
@@ -5508,7 +5528,7 @@
         <v>10</v>
       </c>
       <c r="T74" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
@@ -5516,10 +5536,10 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C75" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E75" t="s">
         <v>10</v>
@@ -5575,10 +5595,10 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C76" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E76" t="s">
         <v>10</v>
@@ -5634,10 +5654,10 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E77" t="s">
         <v>10</v>
@@ -5693,13 +5713,13 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C78" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E78" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F78" t="s">
         <v>10</v>
@@ -5744,7 +5764,7 @@
         <v>10</v>
       </c>
       <c r="T78" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.25">
@@ -5752,34 +5772,34 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C79" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D79" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E79" t="s">
+        <v>27</v>
+      </c>
+      <c r="F79" t="s">
+        <v>146</v>
+      </c>
+      <c r="G79" t="s">
+        <v>10</v>
+      </c>
+      <c r="H79" t="s">
+        <v>10</v>
+      </c>
+      <c r="I79" t="s">
+        <v>10</v>
+      </c>
+      <c r="J79" t="s">
         <v>28</v>
       </c>
-      <c r="F79" t="s">
-        <v>147</v>
-      </c>
-      <c r="G79" t="s">
-        <v>10</v>
-      </c>
-      <c r="H79" t="s">
-        <v>10</v>
-      </c>
-      <c r="I79" t="s">
-        <v>10</v>
-      </c>
-      <c r="J79" t="s">
-        <v>29</v>
-      </c>
       <c r="K79" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L79" t="s">
         <v>10</v>
@@ -5806,7 +5826,7 @@
         <v>10</v>
       </c>
       <c r="T79" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.25">
@@ -5814,13 +5834,13 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C80" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D80" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E80" t="s">
         <v>10</v>
@@ -5841,7 +5861,7 @@
         <v>10</v>
       </c>
       <c r="K80" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L80" t="s">
         <v>10</v>
@@ -5859,7 +5879,7 @@
         <v>10</v>
       </c>
       <c r="Q80" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="R80" t="s">
         <v>10</v>
@@ -5868,7 +5888,7 @@
         <v>10</v>
       </c>
       <c r="T80" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.25">
@@ -5876,34 +5896,34 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C81" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D81" t="s">
+        <v>209</v>
+      </c>
+      <c r="E81" t="s">
+        <v>10</v>
+      </c>
+      <c r="F81" t="s">
+        <v>10</v>
+      </c>
+      <c r="G81" t="s">
+        <v>10</v>
+      </c>
+      <c r="H81" t="s">
+        <v>10</v>
+      </c>
+      <c r="I81" t="s">
+        <v>10</v>
+      </c>
+      <c r="J81" t="s">
         <v>210</v>
       </c>
-      <c r="E81" t="s">
-        <v>10</v>
-      </c>
-      <c r="F81" t="s">
-        <v>10</v>
-      </c>
-      <c r="G81" t="s">
-        <v>10</v>
-      </c>
-      <c r="H81" t="s">
-        <v>10</v>
-      </c>
-      <c r="I81" t="s">
-        <v>10</v>
-      </c>
-      <c r="J81" t="s">
-        <v>211</v>
-      </c>
       <c r="K81" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L81" t="s">
         <v>10</v>
@@ -5921,7 +5941,7 @@
         <v>10</v>
       </c>
       <c r="Q81" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="R81" t="s">
         <v>10</v>
@@ -5930,7 +5950,7 @@
         <v>10</v>
       </c>
       <c r="T81" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.25">
@@ -5938,13 +5958,13 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C82" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D82" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E82" t="s">
         <v>10</v>
@@ -5965,7 +5985,7 @@
         <v>10</v>
       </c>
       <c r="K82" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L82" t="s">
         <v>10</v>
@@ -5983,7 +6003,7 @@
         <v>10</v>
       </c>
       <c r="Q82" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="R82" t="s">
         <v>10</v>
@@ -5992,7 +6012,7 @@
         <v>10</v>
       </c>
       <c r="T82" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.25">
@@ -6000,13 +6020,13 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C83" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D83" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E83" t="s">
         <v>10</v>
@@ -6051,7 +6071,7 @@
         <v>10</v>
       </c>
       <c r="T83" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.25">
@@ -6059,14 +6079,14 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C84" t="s">
+        <v>224</v>
+      </c>
+      <c r="D84" t="s">
         <v>225</v>
       </c>
-      <c r="D84" t="s">
-        <v>226</v>
-      </c>
       <c r="E84" t="s">
         <v>10</v>
       </c>
@@ -6089,7 +6109,7 @@
         <v>10</v>
       </c>
       <c r="L84" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="M84" t="s">
         <v>10</v>
@@ -6113,7 +6133,7 @@
         <v>10</v>
       </c>
       <c r="T84" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.25">
@@ -6121,13 +6141,13 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C85" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D85" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E85" t="s">
         <v>10</v>
@@ -6136,7 +6156,7 @@
         <v>10</v>
       </c>
       <c r="G85" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H85" t="s">
         <v>10</v>
@@ -6172,7 +6192,7 @@
         <v>10</v>
       </c>
       <c r="T85" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.25">
@@ -6180,13 +6200,13 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C86" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D86" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E86" t="s">
         <v>10</v>
@@ -6204,13 +6224,13 @@
         <v>10</v>
       </c>
       <c r="J86" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K86" t="s">
         <v>10</v>
       </c>
       <c r="L86" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M86" t="s">
         <v>10</v>
@@ -6225,7 +6245,7 @@
         <v>10</v>
       </c>
       <c r="Q86" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R86" t="s">
         <v>10</v>
@@ -6234,7 +6254,7 @@
         <v>10</v>
       </c>
       <c r="T86" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.25">
@@ -6242,13 +6262,13 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C87" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D87" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E87" t="s">
         <v>10</v>
@@ -6272,7 +6292,7 @@
         <v>10</v>
       </c>
       <c r="L87" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M87" t="s">
         <v>10</v>
@@ -6296,7 +6316,7 @@
         <v>10</v>
       </c>
       <c r="T87" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.25">
@@ -6304,13 +6324,13 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C88" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D88" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E88" t="s">
         <v>10</v>
@@ -6334,7 +6354,7 @@
         <v>10</v>
       </c>
       <c r="L88" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M88" t="s">
         <v>10</v>
@@ -6358,7 +6378,7 @@
         <v>10</v>
       </c>
       <c r="T88" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.25">
@@ -6366,13 +6386,13 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C89" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D89" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E89" t="s">
         <v>10</v>
@@ -6390,13 +6410,13 @@
         <v>10</v>
       </c>
       <c r="J89" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K89" t="s">
         <v>10</v>
       </c>
       <c r="L89" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M89" t="s">
         <v>10</v>
@@ -6420,7 +6440,7 @@
         <v>10</v>
       </c>
       <c r="T89" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.25">
@@ -6428,13 +6448,13 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C90" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D90" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E90" t="s">
         <v>10</v>
@@ -6458,7 +6478,7 @@
         <v>10</v>
       </c>
       <c r="L90" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M90" t="s">
         <v>10</v>
@@ -6482,7 +6502,7 @@
         <v>10</v>
       </c>
       <c r="T90" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.25">
@@ -6490,16 +6510,16 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C91" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E91" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F91" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G91" t="s">
         <v>10</v>
@@ -6511,10 +6531,10 @@
         <v>10</v>
       </c>
       <c r="J91" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K91" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L91" t="s">
         <v>10</v>
@@ -6523,7 +6543,7 @@
         <v>10</v>
       </c>
       <c r="N91" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="O91" t="s">
         <v>10</v>
@@ -6541,7 +6561,7 @@
         <v>10</v>
       </c>
       <c r="T91" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.25">
@@ -6549,19 +6569,19 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C92" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E92" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F92" t="s">
         <v>10</v>
       </c>
       <c r="G92" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H92" t="s">
         <v>10</v>
@@ -6570,20 +6590,20 @@
         <v>10</v>
       </c>
       <c r="J92" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K92" t="s">
+        <v>209</v>
+      </c>
+      <c r="L92" t="s">
         <v>210</v>
       </c>
-      <c r="L92" t="s">
+      <c r="M92" t="s">
+        <v>10</v>
+      </c>
+      <c r="N92" t="s">
         <v>211</v>
       </c>
-      <c r="M92" t="s">
-        <v>10</v>
-      </c>
-      <c r="N92" t="s">
-        <v>212</v>
-      </c>
       <c r="O92" t="s">
         <v>10</v>
       </c>
@@ -6600,7 +6620,7 @@
         <v>10</v>
       </c>
       <c r="T92" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.25">
@@ -6608,7 +6628,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E93" t="s">
         <v>10</v>
@@ -6617,19 +6637,19 @@
         <v>10</v>
       </c>
       <c r="G93" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H93" t="s">
         <v>10</v>
       </c>
       <c r="I93" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J93" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K93" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L93" t="s">
         <v>10</v>
@@ -6656,7 +6676,7 @@
         <v>10</v>
       </c>
       <c r="T93" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.25">
@@ -6664,7 +6684,13 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="C94" t="s">
+        <v>281</v>
+      </c>
+      <c r="D94" t="s">
+        <v>160</v>
       </c>
       <c r="E94" t="s">
         <v>10</v>
@@ -6673,13 +6699,13 @@
         <v>10</v>
       </c>
       <c r="G94" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H94" t="s">
         <v>10</v>
       </c>
       <c r="I94" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J94" t="s">
         <v>10</v>
@@ -6688,7 +6714,7 @@
         <v>10</v>
       </c>
       <c r="L94" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M94" t="s">
         <v>10</v>
@@ -6712,7 +6738,7 @@
         <v>10</v>
       </c>
       <c r="T94" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.25">
@@ -6720,7 +6746,13 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="C95" t="s">
+        <v>282</v>
+      </c>
+      <c r="D95" t="s">
+        <v>155</v>
       </c>
       <c r="E95" t="s">
         <v>10</v>
@@ -6729,13 +6761,13 @@
         <v>10</v>
       </c>
       <c r="G95" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H95" t="s">
         <v>10</v>
       </c>
       <c r="I95" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J95" t="s">
         <v>10</v>
@@ -6744,7 +6776,7 @@
         <v>10</v>
       </c>
       <c r="L95" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M95" t="s">
         <v>10</v>
@@ -6768,7 +6800,7 @@
         <v>10</v>
       </c>
       <c r="T95" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.25">
@@ -6835,47 +6867,47 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
+        <v>47</v>
+      </c>
+      <c r="E97" t="s">
+        <v>10</v>
+      </c>
+      <c r="F97" t="s">
+        <v>10</v>
+      </c>
+      <c r="G97" t="s">
         <v>48</v>
       </c>
-      <c r="E97" t="s">
-        <v>10</v>
-      </c>
-      <c r="F97" t="s">
-        <v>10</v>
-      </c>
-      <c r="G97" t="s">
+      <c r="H97" t="s">
+        <v>168</v>
+      </c>
+      <c r="I97" t="s">
+        <v>206</v>
+      </c>
+      <c r="J97" t="s">
+        <v>10</v>
+      </c>
+      <c r="K97" t="s">
+        <v>10</v>
+      </c>
+      <c r="L97" t="s">
+        <v>10</v>
+      </c>
+      <c r="M97" t="s">
+        <v>10</v>
+      </c>
+      <c r="N97" t="s">
+        <v>10</v>
+      </c>
+      <c r="O97" t="s">
+        <v>10</v>
+      </c>
+      <c r="P97" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q97" t="s">
         <v>49</v>
       </c>
-      <c r="H97" t="s">
-        <v>169</v>
-      </c>
-      <c r="I97" t="s">
-        <v>207</v>
-      </c>
-      <c r="J97" t="s">
-        <v>10</v>
-      </c>
-      <c r="K97" t="s">
-        <v>10</v>
-      </c>
-      <c r="L97" t="s">
-        <v>10</v>
-      </c>
-      <c r="M97" t="s">
-        <v>10</v>
-      </c>
-      <c r="N97" t="s">
-        <v>10</v>
-      </c>
-      <c r="O97" t="s">
-        <v>10</v>
-      </c>
-      <c r="P97" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q97" t="s">
-        <v>50</v>
-      </c>
       <c r="R97" t="s">
         <v>10</v>
       </c>
@@ -6883,7 +6915,7 @@
         <v>10</v>
       </c>
       <c r="T97" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.25">
@@ -6891,47 +6923,47 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
+        <v>50</v>
+      </c>
+      <c r="E98" t="s">
+        <v>10</v>
+      </c>
+      <c r="F98" t="s">
+        <v>10</v>
+      </c>
+      <c r="G98" t="s">
+        <v>18</v>
+      </c>
+      <c r="H98" t="s">
+        <v>204</v>
+      </c>
+      <c r="I98" t="s">
+        <v>207</v>
+      </c>
+      <c r="J98" t="s">
+        <v>184</v>
+      </c>
+      <c r="K98" t="s">
+        <v>10</v>
+      </c>
+      <c r="L98" t="s">
+        <v>10</v>
+      </c>
+      <c r="M98" t="s">
+        <v>10</v>
+      </c>
+      <c r="N98" t="s">
+        <v>10</v>
+      </c>
+      <c r="O98" t="s">
+        <v>10</v>
+      </c>
+      <c r="P98" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q98" t="s">
         <v>51</v>
       </c>
-      <c r="E98" t="s">
-        <v>10</v>
-      </c>
-      <c r="F98" t="s">
-        <v>10</v>
-      </c>
-      <c r="G98" t="s">
-        <v>19</v>
-      </c>
-      <c r="H98" t="s">
-        <v>205</v>
-      </c>
-      <c r="I98" t="s">
-        <v>208</v>
-      </c>
-      <c r="J98" t="s">
-        <v>185</v>
-      </c>
-      <c r="K98" t="s">
-        <v>10</v>
-      </c>
-      <c r="L98" t="s">
-        <v>10</v>
-      </c>
-      <c r="M98" t="s">
-        <v>10</v>
-      </c>
-      <c r="N98" t="s">
-        <v>10</v>
-      </c>
-      <c r="O98" t="s">
-        <v>10</v>
-      </c>
-      <c r="P98" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q98" t="s">
-        <v>52</v>
-      </c>
       <c r="R98" t="s">
         <v>10</v>
       </c>
@@ -6939,7 +6971,7 @@
         <v>10</v>
       </c>
       <c r="T98" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.25">
@@ -6947,7 +6979,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E99" t="s">
         <v>10</v>
@@ -6956,7 +6988,7 @@
         <v>10</v>
       </c>
       <c r="G99" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H99" t="s">
         <v>10</v>
@@ -6995,7 +7027,7 @@
         <v>10</v>
       </c>
       <c r="T99" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.25">
@@ -7003,13 +7035,13 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E100" t="s">
         <v>10</v>
       </c>
       <c r="F100" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G100" t="s">
         <v>10</v>
@@ -7051,7 +7083,7 @@
         <v>10</v>
       </c>
       <c r="T100" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.25">
@@ -7059,10 +7091,10 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C101" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E101" t="s">
         <v>10</v>
@@ -7118,10 +7150,10 @@
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C102" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E102" t="s">
         <v>10</v>
@@ -7198,111 +7230,111 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B11" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated relays to use 1000VDC switched versions. removed discharge main realy.
</commit_message>
<xml_diff>
--- a/board/crossBar.xlsx
+++ b/board/crossBar.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1841" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1839" uniqueCount="284">
   <si>
     <t>AF0</t>
   </si>
@@ -850,9 +850,6 @@
   </si>
   <si>
     <t>CHG_RELAY</t>
-  </si>
-  <si>
-    <t>DISCHG_RELAY_MAIN</t>
   </si>
   <si>
     <t>OPTO_SIGNAL_RELAY</t>
@@ -1226,7 +1223,7 @@
       <selection activeCell="G2" sqref="G2"/>
       <selection pane="topRight" activeCell="G2" sqref="G2"/>
       <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
-      <selection pane="bottomRight" activeCell="C94" sqref="C94"/>
+      <selection pane="bottomRight" activeCell="C88" sqref="C88:D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2752,7 +2749,7 @@
         <v>98</v>
       </c>
       <c r="C27" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D27" t="s">
         <v>177</v>
@@ -2814,7 +2811,7 @@
         <v>99</v>
       </c>
       <c r="C28" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D28" t="s">
         <v>176</v>
@@ -6144,7 +6141,7 @@
         <v>139</v>
       </c>
       <c r="C85" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D85" t="s">
         <v>225</v>
@@ -6203,7 +6200,7 @@
         <v>67</v>
       </c>
       <c r="C86" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D86" t="s">
         <v>225</v>
@@ -6327,7 +6324,7 @@
         <v>68</v>
       </c>
       <c r="C88" t="s">
-        <v>278</v>
+        <v>226</v>
       </c>
       <c r="D88" t="s">
         <v>225</v>
@@ -6389,7 +6386,7 @@
         <v>69</v>
       </c>
       <c r="C89" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D89" t="s">
         <v>225</v>
@@ -6450,12 +6447,6 @@
       <c r="B90" t="s">
         <v>70</v>
       </c>
-      <c r="C90" t="s">
-        <v>227</v>
-      </c>
-      <c r="D90" t="s">
-        <v>225</v>
-      </c>
       <c r="E90" t="s">
         <v>10</v>
       </c>
@@ -6687,7 +6678,7 @@
         <v>45</v>
       </c>
       <c r="C94" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D94" t="s">
         <v>160</v>
@@ -6749,7 +6740,7 @@
         <v>46</v>
       </c>
       <c r="C95" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D95" t="s">
         <v>155</v>

</xml_diff>